<commit_message>
Ajuste de avalucion del modelo.
graficar_datos - grafica originales vs prediccion
ejecutar_prueba_modelo - ejecuta el modelo
</commit_message>
<xml_diff>
--- a/PreparacionDatos/FloraTotal_3mes_4V.xlsx
+++ b/PreparacionDatos/FloraTotal_3mes_4V.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\GitHub\LTSM_Cali\PreparacionDatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68F1E6-50B9-4577-AAA8-15CBA4AD518D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FloraTotal" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>PM10</t>
   </si>
@@ -26,13 +33,316 @@
   </si>
   <si>
     <t>Poblacion</t>
+  </si>
+  <si>
+    <t>[[0.27059582]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.24523598]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.23982777]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25386995]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2400872 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25020882]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2499968 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2585075 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.23780487]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2544364 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2399233 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25410965]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.24701735]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25116652]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.24470167]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26017472]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25201532]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2528668 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25503308]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2592055 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2553138 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2546236 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25080097]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25144804]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2615448 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2610121 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25342965]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2622572 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25366223]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2613088 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2597784 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26308098]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.31063557]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.31052843]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.30250823]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.30701396]]</t>
+  </si>
+  <si>
+    <t>0     24.953753</t>
+  </si>
+  <si>
+    <t>1     19.868654</t>
+  </si>
+  <si>
+    <t>2     27.656900</t>
+  </si>
+  <si>
+    <t>3     26.076992</t>
+  </si>
+  <si>
+    <t>4     27.081070</t>
+  </si>
+  <si>
+    <t>5     24.417490</t>
+  </si>
+  <si>
+    <t>6     33.543011</t>
+  </si>
+  <si>
+    <t>7     26.189116</t>
+  </si>
+  <si>
+    <t>8     28.528126</t>
+  </si>
+  <si>
+    <t>9     16.134058</t>
+  </si>
+  <si>
+    <t>10    28.120001</t>
+  </si>
+  <si>
+    <t>11    25.519133</t>
+  </si>
+  <si>
+    <t>12    19.838018</t>
+  </si>
+  <si>
+    <t>13    22.679886</t>
+  </si>
+  <si>
+    <t>14    18.081238</t>
+  </si>
+  <si>
+    <t>15    31.919754</t>
+  </si>
+  <si>
+    <t>16    47.482609</t>
+  </si>
+  <si>
+    <t>17    38.531296</t>
+  </si>
+  <si>
+    <t>18    47.904537</t>
+  </si>
+  <si>
+    <t>19    46.285915</t>
+  </si>
+  <si>
+    <t>20    35.878597</t>
+  </si>
+  <si>
+    <t>21    32.421597</t>
+  </si>
+  <si>
+    <t>22    27.916824</t>
+  </si>
+  <si>
+    <t>23    37.520321</t>
+  </si>
+  <si>
+    <t>24    35.772816</t>
+  </si>
+  <si>
+    <t>25    34.026611</t>
+  </si>
+  <si>
+    <t>26    31.355671</t>
+  </si>
+  <si>
+    <t>27    22.212193</t>
+  </si>
+  <si>
+    <t>28    20.680435</t>
+  </si>
+  <si>
+    <t>29    25.191208</t>
+  </si>
+  <si>
+    <t>30    28.905861</t>
+  </si>
+  <si>
+    <t>31    28.345888</t>
+  </si>
+  <si>
+    <t>Orginal</t>
+  </si>
+  <si>
+    <t>[[0.27506712]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2506277 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.24541579]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2589483 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2520089 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26190224]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26169518]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26999962]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25646883]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.27294523]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.25857353]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.27262253]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.27232087]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.27647293]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.26999927]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.28545415]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2838665 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.28472456]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2869053 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.29109594]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2936679 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.29296842]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.28908667]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.2897447 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.30595833]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.3054188 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.29770702]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.3066795 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.30344605]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.31125528]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.3096978 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.31305557]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +357,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,10 +400,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -95,11 +414,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -141,7 +468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,9 +500,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,6 +552,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,14 +745,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,97 +772,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>24.9537525177002</v>
+        <v>24.953752517700199</v>
       </c>
       <c r="C2">
         <v>348066</v>
       </c>
       <c r="D2">
-        <v>0.9396125674247742</v>
+        <v>0.93961256742477417</v>
       </c>
       <c r="E2">
         <v>2244668</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>19.86865425109863</v>
+        <v>19.868654251098601</v>
       </c>
       <c r="C3">
         <v>348066</v>
       </c>
       <c r="D3">
-        <v>0.3828134536743164</v>
+        <v>0.38281345367431641</v>
       </c>
       <c r="E3">
         <v>2244668</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>27.65690040588379</v>
+        <v>27.656900405883789</v>
       </c>
       <c r="C4">
         <v>348066</v>
       </c>
       <c r="D4">
-        <v>0.263171911239624</v>
+        <v>0.26317191123962402</v>
       </c>
       <c r="E4">
         <v>2244668</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>26.07699203491211</v>
+        <v>26.076992034912109</v>
       </c>
       <c r="C5">
         <v>348066</v>
       </c>
       <c r="D5">
-        <v>0.5728340148925781</v>
+        <v>0.57283401489257813</v>
       </c>
       <c r="E5">
         <v>2244668</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>27.08106994628906</v>
+        <v>27.081069946289059</v>
       </c>
       <c r="C6">
         <v>391327</v>
       </c>
       <c r="D6">
-        <v>0.1903815716505051</v>
+        <v>0.19038157165050509</v>
       </c>
       <c r="E6">
         <v>2269653</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>24.41749000549316</v>
+        <v>24.417490005493161</v>
       </c>
       <c r="C7">
         <v>391327</v>
@@ -505,29 +874,29 @@
         <v>2269653</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>33.54301071166992</v>
+        <v>33.543010711669922</v>
       </c>
       <c r="C8">
         <v>391327</v>
       </c>
       <c r="D8">
-        <v>0.4089337587356567</v>
+        <v>0.40893375873565668</v>
       </c>
       <c r="E8">
         <v>2269653</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>26.18911552429199</v>
+        <v>26.189115524291989</v>
       </c>
       <c r="C9">
         <v>391327</v>
@@ -539,7 +908,7 @@
         <v>2269653</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -550,13 +919,13 @@
         <v>438769</v>
       </c>
       <c r="D10">
-        <v>0.06072916463017464</v>
+        <v>6.0729164630174637E-2</v>
       </c>
       <c r="E10">
         <v>2294653</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -567,81 +936,81 @@
         <v>438769</v>
       </c>
       <c r="D11">
-        <v>0.4269565045833588</v>
+        <v>0.42695650458335882</v>
       </c>
       <c r="E11">
         <v>2294653</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>28.1200008392334</v>
+        <v>28.120000839233398</v>
       </c>
       <c r="C12">
         <v>438769</v>
       </c>
       <c r="D12">
-        <v>0.1077073141932487</v>
+        <v>0.10770731419324869</v>
       </c>
       <c r="E12">
         <v>2294653</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>25.51913261413574</v>
+        <v>25.519132614135739</v>
       </c>
       <c r="C13">
         <v>438769</v>
       </c>
       <c r="D13">
-        <v>0.4198056757450104</v>
+        <v>0.41980567574501038</v>
       </c>
       <c r="E13">
         <v>2294653</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>19.8380184173584</v>
+        <v>19.838018417358398</v>
       </c>
       <c r="C14">
         <v>484119</v>
       </c>
       <c r="D14">
-        <v>0.1851062774658203</v>
+        <v>0.18510627746582031</v>
       </c>
       <c r="E14">
         <v>2319684</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>22.67988586425781</v>
+        <v>22.679885864257809</v>
       </c>
       <c r="C15">
         <v>484119</v>
       </c>
       <c r="D15">
-        <v>0.2761108577251434</v>
+        <v>0.27611085772514338</v>
       </c>
       <c r="E15">
         <v>2319684</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -658,46 +1027,46 @@
         <v>2319684</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>31.91975402832031</v>
+        <v>31.919754028320309</v>
       </c>
       <c r="C17">
         <v>484119</v>
       </c>
       <c r="D17">
-        <v>0.4728686213493347</v>
+        <v>0.47286862134933472</v>
       </c>
       <c r="E17">
         <v>2319684</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>47.48260879516602</v>
+        <v>47.482608795166023</v>
       </c>
       <c r="C18">
         <v>526339</v>
       </c>
       <c r="D18">
-        <v>0.2156473398208618</v>
+        <v>0.21564733982086179</v>
       </c>
       <c r="E18">
         <v>2344734</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>38.53129577636719</v>
+        <v>38.531295776367188</v>
       </c>
       <c r="C19">
         <v>526339</v>
@@ -709,80 +1078,80 @@
         <v>2344734</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>47.90453720092773</v>
+        <v>47.904537200927727</v>
       </c>
       <c r="C20">
         <v>526339</v>
       </c>
       <c r="D20">
-        <v>0.2815548181533813</v>
+        <v>0.28155481815338129</v>
       </c>
       <c r="E20">
         <v>2344734</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>46.28591537475586</v>
+        <v>46.285915374755859</v>
       </c>
       <c r="C21">
         <v>526339</v>
       </c>
       <c r="D21">
-        <v>0.3724905550479889</v>
+        <v>0.37249055504798889</v>
       </c>
       <c r="E21">
         <v>2344734</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>35.87859725952148</v>
+        <v>35.878597259521477</v>
       </c>
       <c r="C22">
         <v>567353</v>
       </c>
       <c r="D22">
-        <v>0.2085458934307098</v>
+        <v>0.20854589343070981</v>
       </c>
       <c r="E22">
         <v>2369821</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>32.42159652709961</v>
+        <v>32.421596527099609</v>
       </c>
       <c r="C23">
         <v>567353</v>
       </c>
       <c r="D23">
-        <v>0.1935021430253983</v>
+        <v>0.19350214302539831</v>
       </c>
       <c r="E23">
         <v>2369821</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>27.91682434082031</v>
+        <v>27.916824340820309</v>
       </c>
       <c r="C24">
         <v>567353</v>
@@ -794,12 +1163,12 @@
         <v>2369821</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>37.52032089233398</v>
+        <v>37.520320892333977</v>
       </c>
       <c r="C25">
         <v>567353</v>
@@ -811,24 +1180,24 @@
         <v>2369821</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>35.7728157043457</v>
+        <v>35.772815704345703</v>
       </c>
       <c r="C26">
         <v>601794</v>
       </c>
       <c r="D26">
-        <v>0.2653607130050659</v>
+        <v>0.26536071300506592</v>
       </c>
       <c r="E26">
         <v>2394925</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -839,69 +1208,69 @@
         <v>601794</v>
       </c>
       <c r="D27">
-        <v>0.253803163766861</v>
+        <v>0.25380316376686102</v>
       </c>
       <c r="E27">
         <v>2394925</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>31.35567092895508</v>
+        <v>31.355670928955082</v>
       </c>
       <c r="C28">
         <v>601794</v>
       </c>
       <c r="D28">
-        <v>0.08891304582357407</v>
+        <v>8.8913045823574066E-2</v>
       </c>
       <c r="E28">
         <v>2394925</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>22.21219253540039</v>
+        <v>22.212192535400391</v>
       </c>
       <c r="C29">
         <v>601794</v>
       </c>
       <c r="D29">
-        <v>0.2808128595352173</v>
+        <v>0.28081285953521729</v>
       </c>
       <c r="E29">
         <v>2394925</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>20.68043518066406</v>
+        <v>20.680435180664059</v>
       </c>
       <c r="C30">
         <v>630478</v>
       </c>
       <c r="D30">
-        <v>0.01570048369467258</v>
+        <v>1.5700483694672581E-2</v>
       </c>
       <c r="E30">
         <v>2420114</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>25.19120788574219</v>
+        <v>25.191207885742191</v>
       </c>
       <c r="C31">
         <v>630478</v>
@@ -913,7 +1282,7 @@
         <v>2420114</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -930,12 +1299,12 @@
         <v>2420114</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>28.34588813781738</v>
+        <v>28.345888137817379</v>
       </c>
       <c r="C33">
         <v>630478</v>
@@ -950,4 +1319,412 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEC9D8F-D4E1-43C5-AB61-9D7136B74EC0}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1">
+        <v>36</v>
+      </c>
+      <c r="C1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>